<commit_message>
idw pt.2 2018 - melhor com SUBestimação à mesma - adicionar viés???? experimentar outros k e p
</commit_message>
<xml_diff>
--- a/apa/longatable2018.xlsx
+++ b/apa/longatable2018.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,508 +456,530 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B2" t="n">
-        <v>3101</v>
+        <v>1054</v>
       </c>
       <c r="C2" t="n">
-        <v>11.125</v>
+        <v>13.68181818181818</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B3" t="n">
-        <v>1054</v>
+        <v>3093</v>
       </c>
       <c r="C3" t="n">
-        <v>9.458333333333334</v>
+        <v>36.49166666666667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B4" t="n">
-        <v>3093</v>
+        <v>2017</v>
       </c>
       <c r="C4" t="n">
-        <v>10.30416666666667</v>
+        <v>27.125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B5" t="n">
-        <v>2017</v>
+        <v>3075</v>
       </c>
       <c r="C5" t="n">
-        <v>16.08333333333333</v>
+        <v>48.41666666666666</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B6" t="n">
-        <v>3075</v>
+        <v>1053</v>
       </c>
       <c r="C6" t="n">
-        <v>13.22083333333333</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B7" t="n">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C7" t="n">
-        <v>9.454545454545455</v>
+        <v>24.45454545454545</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B8" t="n">
-        <v>1052</v>
+        <v>3104</v>
       </c>
       <c r="C8" t="n">
-        <v>6.565217391304348</v>
+        <v>41.12380952380953</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B9" t="n">
         <v>5012</v>
       </c>
       <c r="C9" t="n">
-        <v>14.81</v>
+        <v>14.45833333333333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B10" t="n">
         <v>3096</v>
       </c>
       <c r="C10" t="n">
-        <v>8.529166666666667</v>
+        <v>29.04583333333333</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B11" t="n">
-        <v>1046</v>
+        <v>2006</v>
       </c>
       <c r="C11" t="n">
-        <v>15.5</v>
+        <v>37.58333333333334</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B12" t="n">
-        <v>5011</v>
+        <v>1046</v>
       </c>
       <c r="C12" t="n">
-        <v>20.07727272727273</v>
+        <v>18.83333333333333</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B13" t="n">
-        <v>1024</v>
+        <v>5011</v>
       </c>
       <c r="C13" t="n">
-        <v>9.826086956521738</v>
+        <v>38.29166666666666</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B14" t="n">
         <v>1048</v>
       </c>
       <c r="C14" t="n">
-        <v>5.916666666666667</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B15" t="n">
-        <v>2019</v>
+        <v>3072</v>
       </c>
       <c r="C15" t="n">
-        <v>36.66666666666666</v>
+        <v>40.19583333333333</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B16" t="n">
-        <v>3095</v>
+        <v>1023</v>
       </c>
       <c r="C16" t="n">
-        <v>21.97083333333333</v>
+        <v>27.20833333333333</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B17" t="n">
-        <v>2004</v>
+        <v>2019</v>
       </c>
       <c r="C17" t="n">
-        <v>8.666666666666666</v>
+        <v>31.45833333333333</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B18" t="n">
-        <v>3099</v>
+        <v>3095</v>
       </c>
       <c r="C18" t="n">
-        <v>5.983333333333333</v>
+        <v>35.2875</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B19" t="n">
-        <v>3103</v>
+        <v>2004</v>
       </c>
       <c r="C19" t="n">
-        <v>13.31666666666667</v>
+        <v>17.89473684210526</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B20" t="n">
-        <v>1041</v>
+        <v>3099</v>
       </c>
       <c r="C20" t="n">
-        <v>12.66666666666667</v>
+        <v>38.3375</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B21" t="n">
-        <v>1042</v>
+        <v>2021</v>
       </c>
       <c r="C21" t="n">
-        <v>2.208333333333333</v>
+        <v>14.47368421052632</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B22" t="n">
-        <v>2020</v>
+        <v>1028</v>
       </c>
       <c r="C22" t="n">
-        <v>4.125</v>
+        <v>17.22727272727273</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B23" t="n">
-        <v>2018</v>
+        <v>1042</v>
       </c>
       <c r="C23" t="n">
-        <v>14.25</v>
+        <v>10.08333333333333</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B24" t="n">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="C24" t="n">
-        <v>5.958333333333333</v>
+        <v>18.41666666666667</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B25" t="n">
-        <v>1030</v>
+        <v>2018</v>
       </c>
       <c r="C25" t="n">
-        <v>12.75</v>
+        <v>32.83333333333334</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B26" t="n">
-        <v>5007</v>
+        <v>2016</v>
       </c>
       <c r="C26" t="n">
-        <v>10.64583333333333</v>
+        <v>28.45833333333333</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B27" t="n">
-        <v>3083</v>
+        <v>1030</v>
       </c>
       <c r="C27" t="n">
-        <v>11.4125</v>
+        <v>27.28571428571428</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B28" t="n">
-        <v>3085</v>
+        <v>5007</v>
       </c>
       <c r="C28" t="n">
-        <v>8.920833333333333</v>
+        <v>30.44166666666667</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B29" t="n">
-        <v>3102</v>
+        <v>3083</v>
       </c>
       <c r="C29" t="n">
-        <v>6.1875</v>
+        <v>38.62916666666667</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B30" t="n">
-        <v>5008</v>
+        <v>3055</v>
       </c>
       <c r="C30" t="n">
-        <v>15.86666666666667</v>
+        <v>39.97916666666666</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B31" t="n">
-        <v>3089</v>
+        <v>3085</v>
       </c>
       <c r="C31" t="n">
-        <v>11.45833333333333</v>
+        <v>25.6375</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B32" t="n">
-        <v>2022</v>
+        <v>3102</v>
       </c>
       <c r="C32" t="n">
-        <v>8</v>
+        <v>25.84583333333333</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B33" t="n">
-        <v>4002</v>
+        <v>5008</v>
       </c>
       <c r="C33" t="n">
-        <v>10.4375</v>
+        <v>43.41666666666666</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B34" t="n">
-        <v>3097</v>
+        <v>1025</v>
       </c>
       <c r="C34" t="n">
-        <v>17.29583333333333</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B35" t="n">
-        <v>3071</v>
+        <v>3089</v>
       </c>
       <c r="C35" t="n">
-        <v>9.191666666666666</v>
+        <v>27.72083333333333</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B36" t="n">
-        <v>1044</v>
+        <v>1051</v>
       </c>
       <c r="C36" t="n">
-        <v>13.33333333333333</v>
+        <v>16.58333333333333</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B37" t="n">
-        <v>3063</v>
+        <v>2022</v>
       </c>
       <c r="C37" t="n">
-        <v>14.77916666666667</v>
+        <v>28.625</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B38" t="n">
-        <v>1043</v>
+        <v>3097</v>
       </c>
       <c r="C38" t="n">
-        <v>5.238095238095238</v>
+        <v>43.25416666666666</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B39" t="n">
-        <v>3094</v>
+        <v>3071</v>
       </c>
       <c r="C39" t="n">
-        <v>8.491666666666667</v>
+        <v>36.34166666666667</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B40" t="n">
-        <v>3091</v>
+        <v>1044</v>
       </c>
       <c r="C40" t="n">
-        <v>6.6375</v>
+        <v>27.79166666666667</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B41" t="n">
-        <v>3084</v>
+        <v>3063</v>
       </c>
       <c r="C41" t="n">
-        <v>3.733333333333334</v>
+        <v>38.65833333333333</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B42" t="n">
-        <v>3100</v>
+        <v>1043</v>
       </c>
       <c r="C42" t="n">
-        <v>21.02142857142857</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B43" t="n">
-        <v>4004</v>
+        <v>3094</v>
       </c>
       <c r="C43" t="n">
-        <v>30.94117647058824</v>
+        <v>39.85833333333333</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B44" t="n">
-        <v>1055</v>
+        <v>3091</v>
       </c>
       <c r="C44" t="n">
-        <v>9.625</v>
+        <v>28.62916666666667</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B45" t="n">
-        <v>4003</v>
+        <v>3084</v>
       </c>
       <c r="C45" t="n">
-        <v>5.666666666666667</v>
+        <v>31.62083333333333</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B46" t="n">
-        <v>4006</v>
+        <v>1055</v>
       </c>
       <c r="C46" t="n">
-        <v>21.66666666666667</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>43026</v>
+        <v>43271</v>
       </c>
       <c r="B47" t="n">
+        <v>4003</v>
+      </c>
+      <c r="C47" t="n">
+        <v>19.29166666666667</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>43271</v>
+      </c>
+      <c r="B48" t="n">
+        <v>4006</v>
+      </c>
+      <c r="C48" t="n">
+        <v>25.33333333333333</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>43271</v>
+      </c>
+      <c r="B49" t="n">
         <v>1031</v>
       </c>
-      <c r="C47" t="n">
-        <v>10.91666666666667</v>
+      <c r="C49" t="n">
+        <v>25.70588235294118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>